<commit_message>
ERD and Phase plan
Phase plan has extra specifications
</commit_message>
<xml_diff>
--- a/UML/Phase Plan.xlsx
+++ b/UML/Phase Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Desktop\2SemesterPreExamProject\SWC_SWD_ITO\Covid-19-Project\UML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C1F45E-555C-4259-ACBA-190B65A77E9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE61D310-95BB-43A4-A35A-6A7D0E1ACB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3648" yWindow="1356" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5868" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="65">
   <si>
     <t>SWC,SWD,ITO</t>
   </si>
@@ -211,9 +211,6 @@
   </si>
   <si>
     <t>Code &amp; Test</t>
-  </si>
-  <si>
-    <t>Data Base</t>
   </si>
   <si>
     <t>Interation 1</t>
@@ -258,7 +255,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -318,11 +315,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -365,9 +408,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -376,6 +416,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO53"/>
+  <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:AN52"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AO23" sqref="AO23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,12 +740,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="3"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -724,10 +785,10 @@
       <c r="AO1" s="1"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="3"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -767,12 +828,12 @@
       <c r="AO2" s="1"/>
     </row>
     <row r="3" spans="1:41" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="3"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -818,10 +879,10 @@
       <c r="AO3" s="1"/>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="3"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -861,12 +922,12 @@
       <c r="AO4" s="1"/>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="3"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1340,10 +1401,10 @@
       <c r="AO11" s="1"/>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="18"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="4">
         <v>1</v>
       </c>
@@ -1391,10 +1452,10 @@
       <c r="AO12" s="1"/>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="19"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="4">
         <v>1</v>
       </c>
@@ -1602,8 +1663,12 @@
       <c r="C17" s="4">
         <v>1</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="D17" s="5">
+        <v>44331</v>
+      </c>
+      <c r="E17" s="5">
+        <v>44331</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1616,7 +1681,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="R17" s="7"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
@@ -1649,8 +1714,12 @@
       <c r="C18" s="4">
         <v>1</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="D18" s="5">
+        <v>44331</v>
+      </c>
+      <c r="E18" s="5">
+        <v>44331</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1663,7 +1732,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
+      <c r="R18" s="7"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
@@ -1696,8 +1765,12 @@
       <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="D19" s="5">
+        <v>44331</v>
+      </c>
+      <c r="E19" s="5">
+        <v>44331</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1710,7 +1783,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
+      <c r="R19" s="7"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
@@ -1743,8 +1816,12 @@
       <c r="C20" s="4">
         <v>1</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="D20" s="5">
+        <v>44331</v>
+      </c>
+      <c r="E20" s="5">
+        <v>44331</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1757,7 +1834,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
+      <c r="R20" s="7"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
@@ -1829,7 +1906,7 @@
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -1878,10 +1955,14 @@
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="4">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D23" s="5">
+        <v>44332</v>
+      </c>
+      <c r="E23" s="5">
+        <v>44332</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1895,8 +1976,8 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="9"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
@@ -1925,10 +2006,14 @@
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="4">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D24" s="5">
+        <v>44340</v>
+      </c>
+      <c r="E24" s="5">
+        <v>44340</v>
+      </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1950,7 +2035,7 @@
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
-      <c r="AA24" s="1"/>
+      <c r="AA24" s="7"/>
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
@@ -1972,10 +2057,14 @@
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="4">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D25" s="5">
+        <v>44332</v>
+      </c>
+      <c r="E25" s="5">
+        <v>44332</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1989,7 +2078,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
+      <c r="S25" s="26"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
@@ -2021,8 +2110,12 @@
       <c r="C26" s="4">
         <v>1</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="D26" s="5">
+        <v>44332</v>
+      </c>
+      <c r="E26" s="5">
+        <v>44332</v>
+      </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -2036,11 +2129,11 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="29"/>
+      <c r="U26" s="29"/>
+      <c r="V26" s="28"/>
+      <c r="W26" s="9"/>
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
@@ -2066,10 +2159,14 @@
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="4">
-        <v>0</v>
-      </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
+        <v>1</v>
+      </c>
+      <c r="D27" s="5">
+        <v>44333</v>
+      </c>
+      <c r="E27" s="5">
+        <v>44333</v>
+      </c>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
@@ -2084,8 +2181,8 @@
       <c r="Q27" s="13"/>
       <c r="R27" s="13"/>
       <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="13"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="9"/>
       <c r="V27" s="13"/>
       <c r="W27" s="13"/>
       <c r="X27" s="13"/>
@@ -2097,7 +2194,7 @@
       <c r="AD27" s="13"/>
       <c r="AE27" s="13"/>
       <c r="AF27" s="13"/>
-      <c r="AG27" s="13"/>
+      <c r="AG27" s="27"/>
       <c r="AH27" s="13"/>
       <c r="AI27" s="13"/>
       <c r="AJ27" s="13"/>
@@ -2108,309 +2205,483 @@
       <c r="AO27" s="13"/>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="14"/>
+      <c r="A28" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C28" s="4">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
-      <c r="AA28" s="1"/>
-      <c r="AB28" s="1"/>
-      <c r="AC28" s="1"/>
-      <c r="AD28" s="1"/>
-      <c r="AE28" s="1"/>
-      <c r="AF28" s="1"/>
-      <c r="AG28" s="1"/>
-      <c r="AH28" s="1"/>
-      <c r="AI28" s="1"/>
-      <c r="AJ28" s="1"/>
-      <c r="AK28" s="1"/>
-      <c r="AL28" s="1"/>
-      <c r="AM28" s="1"/>
-      <c r="AN28" s="1"/>
-      <c r="AO28" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D28" s="5">
+        <v>44334</v>
+      </c>
+      <c r="E28" s="5">
+        <v>44334</v>
+      </c>
+      <c r="U28" s="25"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A29" s="17" t="s">
-        <v>64</v>
-      </c>
+      <c r="A29" s="16"/>
       <c r="B29" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5">
+        <v>44335</v>
+      </c>
+      <c r="E29" s="5">
+        <v>44335</v>
+      </c>
+      <c r="V29" s="12"/>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C30" s="4">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5">
+        <v>44335</v>
+      </c>
+      <c r="E30" s="5">
+        <v>44335</v>
+      </c>
+      <c r="V30" s="12"/>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5">
+        <v>44335</v>
+      </c>
+      <c r="E31" s="5">
+        <v>44335</v>
+      </c>
+      <c r="V31" s="12"/>
     </row>
     <row r="32" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
+        <v>42</v>
+      </c>
+      <c r="C32" s="4">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5">
+        <v>44335</v>
+      </c>
+      <c r="E32" s="5">
+        <v>44335</v>
+      </c>
+      <c r="V32" s="12"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A33" s="16"/>
       <c r="B33" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="17"/>
+        <v>43</v>
+      </c>
+      <c r="C33" s="4">
+        <v>1</v>
+      </c>
+      <c r="D33" s="5">
+        <v>44335</v>
+      </c>
+      <c r="E33" s="5">
+        <v>44335</v>
+      </c>
+      <c r="V33" s="12"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A34" s="16"/>
       <c r="B34" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="17"/>
+        <v>44</v>
+      </c>
+      <c r="C34" s="4">
+        <v>1</v>
+      </c>
+      <c r="D34" s="5">
+        <v>44336</v>
+      </c>
+      <c r="E34" s="5">
+        <v>44336</v>
+      </c>
+      <c r="W34" s="12"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A35" s="16"/>
       <c r="B35" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="17"/>
+        <v>45</v>
+      </c>
+      <c r="C35" s="4">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5">
+        <v>44336</v>
+      </c>
+      <c r="E35" s="5">
+        <v>44336</v>
+      </c>
+      <c r="W35" s="12"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A36" s="16"/>
       <c r="B36" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="17"/>
+        <v>46</v>
+      </c>
+      <c r="C36" s="4">
+        <v>1</v>
+      </c>
+      <c r="D36" s="5">
+        <v>44337</v>
+      </c>
+      <c r="E36" s="5">
+        <v>44337</v>
+      </c>
+      <c r="X36" s="12"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A37" s="16"/>
       <c r="B37" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="17"/>
+        <v>47</v>
+      </c>
+      <c r="C37" s="4">
+        <v>1</v>
+      </c>
+      <c r="D37" s="5">
+        <v>44337</v>
+      </c>
+      <c r="E37" s="5">
+        <v>44337</v>
+      </c>
+      <c r="X37" s="12"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A38" s="16"/>
       <c r="B38" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="17"/>
+        <v>48</v>
+      </c>
+      <c r="C38" s="4">
+        <v>1</v>
+      </c>
+      <c r="D38" s="5">
+        <v>44337</v>
+      </c>
+      <c r="E38" s="5">
+        <v>44337</v>
+      </c>
+      <c r="X38" s="12"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A39" s="16"/>
       <c r="B39" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="17"/>
+        <v>49</v>
+      </c>
+      <c r="C39" s="4">
+        <v>1</v>
+      </c>
+      <c r="D39" s="5">
+        <v>44337</v>
+      </c>
+      <c r="E39" s="5">
+        <v>44337</v>
+      </c>
+      <c r="X39" s="24"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A40" s="16"/>
       <c r="B40" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="17"/>
+        <v>50</v>
+      </c>
+      <c r="C40" s="4">
+        <v>1</v>
+      </c>
+      <c r="D40" s="5">
+        <v>44337</v>
+      </c>
+      <c r="E40" s="5">
+        <v>44337</v>
+      </c>
+      <c r="X40" s="12"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A41" s="16"/>
       <c r="B41" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="17"/>
+        <v>51</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1</v>
+      </c>
+      <c r="D41" s="5">
+        <v>44337</v>
+      </c>
+      <c r="E41" s="5">
+        <v>44337</v>
+      </c>
+      <c r="X41" s="25"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A42" s="16"/>
       <c r="B42" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="17"/>
+        <v>52</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
+      <c r="D42" s="5">
+        <v>44337</v>
+      </c>
+      <c r="E42" s="5">
+        <v>44337</v>
+      </c>
+      <c r="X42" s="12"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A43" s="16"/>
       <c r="B43" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="17"/>
+        <v>53</v>
+      </c>
+      <c r="C43" s="4">
+        <v>1</v>
+      </c>
+      <c r="D43" s="5">
+        <v>44338</v>
+      </c>
+      <c r="E43" s="5">
+        <v>44338</v>
+      </c>
+      <c r="Y43" s="12"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A44" s="16"/>
       <c r="B44" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="17"/>
+        <v>54</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+      <c r="D44" s="5">
+        <v>44339</v>
+      </c>
+      <c r="E44" s="5">
+        <v>44339</v>
+      </c>
+      <c r="Z44" s="12"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A45" s="16"/>
       <c r="B45" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="17"/>
+        <v>55</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1</v>
+      </c>
+      <c r="D45" s="5">
+        <v>44339</v>
+      </c>
+      <c r="E45" s="5">
+        <v>44339</v>
+      </c>
+      <c r="Z45" s="12"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A46" s="16"/>
       <c r="B46" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="17"/>
+        <v>56</v>
+      </c>
+      <c r="C46" s="4">
+        <v>1</v>
+      </c>
+      <c r="D46" s="5">
+        <v>44339</v>
+      </c>
+      <c r="E46" s="5">
+        <v>44339</v>
+      </c>
+      <c r="Z46" s="12"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A47" s="16"/>
       <c r="B47" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="17"/>
+        <v>57</v>
+      </c>
+      <c r="C47" s="4">
+        <v>1</v>
+      </c>
+      <c r="D47" s="5">
+        <v>44339</v>
+      </c>
+      <c r="E47" s="5">
+        <v>44339</v>
+      </c>
+      <c r="Z47" s="12"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A48" s="16"/>
       <c r="B48" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C48" s="4">
+        <v>1</v>
+      </c>
+      <c r="D48" s="5">
+        <v>44339</v>
+      </c>
+      <c r="E48" s="5">
+        <v>44339</v>
+      </c>
+      <c r="Z48" s="12"/>
     </row>
     <row r="49" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A49" s="17"/>
-      <c r="B49" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="A49" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="14"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="14"/>
+      <c r="R49" s="14"/>
+      <c r="S49" s="14"/>
+      <c r="T49" s="14"/>
+      <c r="U49" s="14"/>
+      <c r="V49" s="14"/>
+      <c r="W49" s="14"/>
+      <c r="X49" s="14"/>
+      <c r="Y49" s="14"/>
+      <c r="Z49" s="14"/>
+      <c r="AA49" s="14"/>
+      <c r="AB49" s="14"/>
+      <c r="AC49" s="14"/>
+      <c r="AD49" s="14"/>
+      <c r="AE49" s="14"/>
+      <c r="AF49" s="14"/>
+      <c r="AG49" s="14"/>
+      <c r="AH49" s="14"/>
+      <c r="AI49" s="14"/>
+      <c r="AJ49" s="14"/>
+      <c r="AK49" s="14"/>
+      <c r="AL49" s="14"/>
+      <c r="AM49" s="14"/>
+      <c r="AN49" s="14"/>
     </row>
     <row r="50" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="14"/>
-      <c r="O50" s="14"/>
-      <c r="P50" s="14"/>
-      <c r="Q50" s="14"/>
-      <c r="R50" s="14"/>
-      <c r="S50" s="14"/>
-      <c r="T50" s="14"/>
-      <c r="U50" s="14"/>
-      <c r="V50" s="14"/>
-      <c r="W50" s="14"/>
-      <c r="X50" s="14"/>
-      <c r="Y50" s="14"/>
-      <c r="Z50" s="14"/>
-      <c r="AA50" s="14"/>
-      <c r="AB50" s="14"/>
-      <c r="AC50" s="14"/>
-      <c r="AD50" s="14"/>
-      <c r="AE50" s="14"/>
-      <c r="AF50" s="14"/>
-      <c r="AG50" s="14"/>
-      <c r="AH50" s="14"/>
-      <c r="AI50" s="14"/>
-      <c r="AJ50" s="14"/>
-      <c r="AK50" s="14"/>
-      <c r="AL50" s="14"/>
-      <c r="AM50" s="14"/>
-      <c r="AN50" s="14"/>
+      <c r="C50" s="23">
+        <v>1</v>
+      </c>
+      <c r="D50" s="5">
+        <v>44332</v>
+      </c>
+      <c r="E50" s="5">
+        <v>44348</v>
+      </c>
+      <c r="S50" s="20"/>
+      <c r="T50" s="21"/>
+      <c r="U50" s="21"/>
+      <c r="V50" s="21"/>
+      <c r="W50" s="21"/>
+      <c r="X50" s="21"/>
+      <c r="Y50" s="21"/>
+      <c r="Z50" s="21"/>
+      <c r="AA50" s="21"/>
+      <c r="AB50" s="21"/>
+      <c r="AC50" s="21"/>
+      <c r="AD50" s="21"/>
+      <c r="AE50" s="21"/>
+      <c r="AF50" s="21"/>
+      <c r="AG50" s="21"/>
+      <c r="AH50" s="21"/>
+      <c r="AI50" s="22"/>
     </row>
     <row r="51" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="14"/>
+      <c r="O51" s="14"/>
+      <c r="P51" s="14"/>
+      <c r="Q51" s="14"/>
+      <c r="R51" s="14"/>
+      <c r="S51" s="14"/>
+      <c r="T51" s="14"/>
+      <c r="U51" s="14"/>
+      <c r="V51" s="14"/>
+      <c r="W51" s="14"/>
+      <c r="X51" s="14"/>
+      <c r="Y51" s="14"/>
+      <c r="Z51" s="14"/>
+      <c r="AA51" s="14"/>
+      <c r="AB51" s="14"/>
+      <c r="AC51" s="14"/>
+      <c r="AD51" s="14"/>
+      <c r="AE51" s="14"/>
+      <c r="AF51" s="14"/>
+      <c r="AG51" s="14"/>
+      <c r="AH51" s="14"/>
+      <c r="AI51" s="14"/>
+      <c r="AJ51" s="14"/>
+      <c r="AK51" s="14"/>
+      <c r="AL51" s="14"/>
+      <c r="AM51" s="14"/>
+      <c r="AN51" s="14"/>
     </row>
     <row r="52" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A52" s="14" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
-      <c r="P52" s="14"/>
-      <c r="Q52" s="14"/>
-      <c r="R52" s="14"/>
-      <c r="S52" s="14"/>
-      <c r="T52" s="14"/>
-      <c r="U52" s="14"/>
-      <c r="V52" s="14"/>
-      <c r="W52" s="14"/>
-      <c r="X52" s="14"/>
-      <c r="Y52" s="14"/>
-      <c r="Z52" s="14"/>
-      <c r="AA52" s="14"/>
-      <c r="AB52" s="14"/>
-      <c r="AC52" s="14"/>
-      <c r="AD52" s="14"/>
-      <c r="AE52" s="14"/>
-      <c r="AF52" s="14"/>
-      <c r="AG52" s="14"/>
-      <c r="AH52" s="14"/>
-      <c r="AI52" s="14"/>
-      <c r="AJ52" s="14"/>
-      <c r="AK52" s="14"/>
-      <c r="AL52" s="14"/>
-      <c r="AM52" s="14"/>
-      <c r="AN52" s="14"/>
-    </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A53" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B53" s="14"/>
-      <c r="C53" s="4">
+      <c r="C52" s="4">
         <v>0</v>
       </c>
-      <c r="AJ53" s="12"/>
+      <c r="AJ52" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A9:AN9"/>
-    <mergeCell ref="A21:AN21"/>
-    <mergeCell ref="A50:AN50"/>
-    <mergeCell ref="A52:AN52"/>
-    <mergeCell ref="A22:AN22"/>
-    <mergeCell ref="A29:A49"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
+  <mergeCells count="38">
+    <mergeCell ref="AA6:AG6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AH6:AN6"/>
+    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="Q3:Y3"/>
+    <mergeCell ref="Z3:AM3"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A28:B28"/>
     <mergeCell ref="F6:L6"/>
     <mergeCell ref="M6:S6"/>
     <mergeCell ref="T6:Z6"/>
@@ -2420,13 +2691,27 @@
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A27:B27"/>
-    <mergeCell ref="AA6:AG6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="AH6:AN6"/>
-    <mergeCell ref="H3:P3"/>
-    <mergeCell ref="Q3:Y3"/>
-    <mergeCell ref="Z3:AM3"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A9:AN9"/>
+    <mergeCell ref="A21:AN21"/>
+    <mergeCell ref="A49:AN49"/>
+    <mergeCell ref="A51:AN51"/>
+    <mergeCell ref="A22:AN22"/>
+    <mergeCell ref="A28:A48"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>

</xml_diff>